<commit_message>
Determined the values of accuracy constants for measuring instruments
</commit_message>
<xml_diff>
--- a/01_lab/niepewnosci.xlsx
+++ b/01_lab/niepewnosci.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>amperomierz</t>
   </si>
@@ -57,17 +57,27 @@
   </si>
   <si>
     <t>zakres</t>
+  </si>
+  <si>
+    <t>luksomierz</t>
+  </si>
+  <si>
+    <t>W/m2</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00&quot; &quot;[$zł-415];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$zł-415]"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +85,32 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,17 +130,31 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="171" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
+    <cellStyle name="Heading" xfId="2"/>
+    <cellStyle name="Heading1" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Result" xfId="4"/>
+    <cellStyle name="Result2" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -382,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,7 +445,7 @@
     <col min="7" max="7" width="5.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,13 +464,22 @@
       <c r="H1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2">
+        <v>0.01</v>
+      </c>
+      <c r="C2">
         <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="C2">
-        <v>1E-3</v>
       </c>
       <c r="G2">
         <v>0.01</v>
@@ -428,8 +487,14 @@
       <c r="H2">
         <v>5.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0.05</v>
+      </c>
+      <c r="L2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -442,8 +507,14 @@
       <c r="H3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -459,8 +530,14 @@
       <c r="H4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>200</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -479,14 +556,20 @@
       <c r="H5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>124.3</v>
       </c>
       <c r="B6" s="2">
         <f>B$2*A6+C$2*B$4</f>
-        <v>0.82150000000000012</v>
+        <v>2.2430000000000003</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s">
@@ -502,14 +585,21 @@
       <c r="H6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" s="1">
+        <v>60</v>
+      </c>
+      <c r="K6" s="1">
+        <f>K$2*J6+L$2*K$4</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>169.4</v>
       </c>
       <c r="B7" s="2">
         <f>B$2*A7+C$2*B$4</f>
-        <v>1.0470000000000002</v>
+        <v>2.694</v>
       </c>
       <c r="C7" s="2"/>
       <c r="F7" s="1">
@@ -519,14 +609,21 @@
         <f t="shared" ref="G7:G22" si="0">G$2*F7+H$2*H$4</f>
         <v>0.12620000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J7" s="1">
+        <v>65.2</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" ref="K7:K9" si="1">K$2*J7+L$2*K$4</f>
+        <v>4.26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.2</v>
       </c>
       <c r="B8" s="1">
-        <f>B$2*A8+C$2*C$4</f>
-        <v>2.1000000000000001E-2</v>
+        <f t="shared" ref="B8:B28" si="2">B$2*A8+C$2*C$4</f>
+        <v>0.10200000000000001</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" t="s">
@@ -539,14 +636,21 @@
         <f t="shared" si="0"/>
         <v>0.12609999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" s="1">
+        <v>54.5</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="1"/>
+        <v>3.7250000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.6</v>
       </c>
       <c r="B9" s="1">
-        <f>B$2*A9+C$2*C$4</f>
-        <v>2.3E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.10600000000000001</v>
       </c>
       <c r="C9" s="1"/>
       <c r="F9" s="1">
@@ -556,14 +660,21 @@
         <f t="shared" si="0"/>
         <v>0.12529999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="1">
+        <v>55.8</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="1"/>
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" s="1">
-        <f>B$2*A10+C$2*C$4</f>
-        <v>2.5000000000000001E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.11</v>
       </c>
       <c r="C10" s="1"/>
       <c r="F10" s="1">
@@ -574,13 +685,13 @@
         <v>0.1246</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1.43</v>
       </c>
       <c r="B11" s="1">
-        <f>B$2*A11+C$2*C$4</f>
-        <v>2.7150000000000001E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.11430000000000001</v>
       </c>
       <c r="C11" s="1"/>
       <c r="F11" s="1">
@@ -591,13 +702,13 @@
         <v>0.1237</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1.63</v>
       </c>
       <c r="B12" s="1">
-        <f>B$2*A12+C$2*C$4</f>
-        <v>2.8150000000000001E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.1163</v>
       </c>
       <c r="C12" s="1"/>
       <c r="F12" s="1">
@@ -608,13 +719,13 @@
         <v>0.12330000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1.85</v>
       </c>
       <c r="B13" s="1">
-        <f>B$2*A13+C$2*C$4</f>
-        <v>2.9250000000000002E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.11850000000000001</v>
       </c>
       <c r="C13" s="1"/>
       <c r="F13" s="1">
@@ -625,13 +736,13 @@
         <v>0.12280000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
       <c r="B14" s="1">
-        <f>B$2*A14+C$2*C$4</f>
-        <v>0.03</v>
+        <f t="shared" si="2"/>
+        <v>0.12000000000000001</v>
       </c>
       <c r="C14" s="1"/>
       <c r="F14" s="1">
@@ -642,13 +753,13 @@
         <v>0.1225</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.24</v>
       </c>
       <c r="B15" s="1">
-        <f>B$2*A15+C$2*C$4</f>
-        <v>2.12E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.1024</v>
       </c>
       <c r="C15" s="1"/>
       <c r="F15" s="1">
@@ -659,13 +770,13 @@
         <v>0.12180000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2.4300000000000002</v>
       </c>
       <c r="B16" s="1">
-        <f>B$2*A16+C$2*C$4</f>
-        <v>3.2149999999999998E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.12430000000000001</v>
       </c>
       <c r="C16" s="1"/>
       <c r="F16" s="1">
@@ -681,8 +792,8 @@
         <v>2.69</v>
       </c>
       <c r="B17" s="1">
-        <f>B$2*A17+C$2*C$4</f>
-        <v>3.3450000000000001E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.12690000000000001</v>
       </c>
       <c r="C17" s="1"/>
       <c r="F17" s="1">
@@ -698,8 +809,8 @@
         <v>2.99</v>
       </c>
       <c r="B18" s="1">
-        <f>B$2*A18+C$2*C$4</f>
-        <v>3.4950000000000002E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.12990000000000002</v>
       </c>
       <c r="C18" s="1"/>
       <c r="F18" s="3">
@@ -718,8 +829,8 @@
         <v>3.22</v>
       </c>
       <c r="B19" s="1">
-        <f>B$2*A19+C$2*C$4</f>
-        <v>3.61E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.13220000000000001</v>
       </c>
       <c r="C19" s="1"/>
       <c r="F19" s="3">
@@ -735,8 +846,8 @@
         <v>3.37</v>
       </c>
       <c r="B20" s="1">
-        <f>B$2*A20+C$2*C$4</f>
-        <v>3.6850000000000001E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.13370000000000001</v>
       </c>
       <c r="C20" s="1"/>
       <c r="F20" s="1">
@@ -755,8 +866,8 @@
         <v>3.55</v>
       </c>
       <c r="B21" s="1">
-        <f>B$2*A21+C$2*C$4</f>
-        <v>3.7749999999999999E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.13550000000000001</v>
       </c>
       <c r="C21" s="1"/>
       <c r="F21" s="3">
@@ -775,8 +886,8 @@
         <v>3.59</v>
       </c>
       <c r="B22" s="1">
-        <f>B$2*A22+C$2*C$4</f>
-        <v>3.7949999999999998E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.13590000000000002</v>
       </c>
       <c r="C22" s="1"/>
       <c r="F22" s="1">
@@ -795,8 +906,8 @@
         <v>3.88</v>
       </c>
       <c r="B23" s="1">
-        <f>B$2*A23+C$2*C$4</f>
-        <v>3.9400000000000004E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.13880000000000001</v>
       </c>
       <c r="C23" s="1"/>
       <c r="F23" s="3">
@@ -815,15 +926,15 @@
         <v>4.07</v>
       </c>
       <c r="B24" s="1">
-        <f>B$2*A24+C$2*C$4</f>
-        <v>4.0350000000000004E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.14070000000000002</v>
       </c>
       <c r="C24" s="1"/>
       <c r="F24" s="3">
         <v>1.329</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" ref="G24:G28" si="1">G$2*F24+H$2*G$4</f>
+        <f t="shared" ref="G24:G28" si="3">G$2*F24+H$2*G$4</f>
         <v>2.3289999999999998E-2</v>
       </c>
     </row>
@@ -832,15 +943,15 @@
         <v>4.25</v>
       </c>
       <c r="B25" s="1">
-        <f>B$2*A25+C$2*C$4</f>
-        <v>4.1250000000000002E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.14250000000000002</v>
       </c>
       <c r="C25" s="1"/>
       <c r="F25" s="3">
         <v>1.109</v>
       </c>
       <c r="G25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.1090000000000001E-2</v>
       </c>
     </row>
@@ -849,15 +960,15 @@
         <v>4.41</v>
       </c>
       <c r="B26" s="1">
-        <f>B$2*A26+C$2*C$4</f>
-        <v>4.2050000000000004E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.14410000000000001</v>
       </c>
       <c r="C26" s="1"/>
       <c r="F26" s="3">
         <v>0.79300000000000004</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.7930000000000001E-2</v>
       </c>
     </row>
@@ -866,15 +977,15 @@
         <v>4.5199999999999996</v>
       </c>
       <c r="B27" s="1">
-        <f>B$2*A27+C$2*C$4</f>
-        <v>4.2599999999999999E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.1452</v>
       </c>
       <c r="C27" s="1"/>
       <c r="F27" s="3">
         <v>0.67100000000000004</v>
       </c>
       <c r="G27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.6710000000000003E-2</v>
       </c>
     </row>
@@ -883,15 +994,15 @@
         <v>4.6900000000000004</v>
       </c>
       <c r="B28" s="1">
-        <f>B$2*A28+C$2*C$4</f>
-        <v>4.3450000000000003E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.1469</v>
       </c>
       <c r="C28" s="1"/>
       <c r="F28" s="3">
         <v>0.53</v>
       </c>
       <c r="G28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.5300000000000001E-2</v>
       </c>
     </row>

</xml_diff>